<commit_message>
ITF_BBPS&Benny pdf. and updated Excel parts list
</commit_message>
<xml_diff>
--- a/2024/ITFAmpliferProjectParts.xlsx
+++ b/2024/ITFAmpliferProjectParts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leistimo\Documents\GitHub\IgniteTheirFuture\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6A4667-0A01-4502-85FF-5D9989AF31DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A30F740-478A-47D2-8E5E-C826A3B4DE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0956B9F1-DB6B-4831-93C6-0C87A5FA0738}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>Part Description</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>https://www.amazon.com/hz/wishlist/ls/26B7OYRZQ1VQM/ref=nav_wishlist_lists_3</t>
+  </si>
+  <si>
+    <t>Bluetooth Battery Powered Amplifier (Benny)</t>
+  </si>
+  <si>
+    <t>Rock'in Amplifier</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +312,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08EDC910-8677-44CC-B2F0-1B071ED39F6C}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,561 +662,579 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="B2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>7.5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>2.7</v>
+        <v>0.9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>2.4</v>
+        <v>2.7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1">
-        <v>0.8</v>
+        <v>2.4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>7</v>
+        <v>0.8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>1.25</v>
+        <v>3.5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>30</v>
+        <v>1.25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>10.199999999999999</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.21</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1">
-        <v>9.35</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>0.21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9.35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>7</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>0.12</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1">
-        <f>SUM(C3:C17)</f>
+      <c r="C19" s="1">
+        <f>SUM(C4:C18)</f>
         <v>70.179999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="B21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1">
-        <v>30</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1">
-        <v>2.7</v>
+        <v>1.25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1">
-        <v>6</v>
+        <v>2.7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>3.6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1">
-        <v>16</v>
+        <v>3.6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B32" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C32" s="1">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="1">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="1">
-        <f>SUM(C22:C36)</f>
+      <c r="C38" s="1">
+        <f>SUM(C23:C37)</f>
         <v>136.55000000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B21:D21"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{7BAAD23B-7678-4EBB-9B5A-661293E0F674}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{551F451C-DD03-4493-8EA8-59540528086E}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{25E4BF5A-A49F-480D-8849-CB7A7B9B79BE}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{A173BFB9-ABA9-4930-A528-581312F64ED0}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{1E8A2B7D-CC91-4B8A-8EA3-862EA551A3C4}"/>
-    <hyperlink ref="E10" r:id="rId6" display="https://www.amazon.com/Charger-Cabepow-Adapter-Replacement-Certified/dp/B09MRGLZ3W/ref=asc_df_B09MRGLZ3W/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=647232162671&amp;hvpos=&amp;hvnetw=g&amp;hvrand=8620124500595074403&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1016216&amp;hvtargid=pla-1950936299265&amp;mcid=efa7bf99c3543b43b3072f505e67ee13&amp;th=1" xr:uid="{F23F5859-01CD-4F5B-BC9E-C1111199B558}"/>
-    <hyperlink ref="E11" r:id="rId7" display="https://www.amazon.com/Charging-etguuds-Charger-Compatible-Samsung/dp/B089DM4KDW/ref=sr_1_3?crid=PM2LYP9121C&amp;dib=eyJ2IjoiMSJ9.XnJmpogYmdIy1CTZnxjk3yMJVv7eMnOaBQg168qPbg6U5oBzVS_uVzqHed3j6VZUslJKS891U51XQG6IZpFtGbDnRjf5leMIE9xP_5N2HFzCodmkJezSDly3v388XzfURpFN0ydF60pmJ1lZ-zB8nmVreFKbbjYd7UAbfLXusirgoToJLIWO26UszfL60F7HBmmGClCM5uaaSW1PcT_HPap0fMdBMz-B0UsPJVyDNOk.tPHZhfxNUqnfvIHsdn1pVZLA4syls-WTsZfRm-fcHQ8&amp;dib_tag=se&amp;keywords=usb%2Bc%2Bcable&amp;qid=1711749477&amp;sprefix=usb%2Bc%2Bcable%2Caps%2C146&amp;sr=8-3&amp;th=1" xr:uid="{85953D17-CC4C-4B91-8797-ED80017688ED}"/>
-    <hyperlink ref="E16" r:id="rId8" display="https://www.amazon.com/Stainless-Lengths-Available-Machine-Phillips/dp/B0793D86TB/ref=sr_1_21?crid=WBXT9P6GKIPF&amp;dib=eyJ2IjoiMSJ9.L6mfIE51zTPaywqeH0ar3jIX6WQ-gjM-wgJaUqgZeYVm5ChcscbE_zvlzc-lXdKwxf9_HO6jvI_KGoF38sNgFPWOSFrd3uGKhCrvjnYSEAaH61OiLBITDRwChiGXJiekfmtCUjgUL49s0s2umc79HVGfd0oocHT_SdOYOS862KFDrny6U2l-nYdirsQx8XNAaPfJXyXHHC71KG3dNjIx92lPwWic_wvQ3snGnakzY84.B7kH8YazXzMOwjwJAOCM1rgNsxzpzEb8TZWCjs78Xzc&amp;dib_tag=se&amp;keywords=6%2B32%2Bscrews&amp;qid=1711819989&amp;sprefix=6%2B32%2Bscrews%2Caps%2C132&amp;sr=8-21&amp;th=1" xr:uid="{E382410B-BB8A-4CFF-8C9E-BDC4985067E7}"/>
-    <hyperlink ref="E22" r:id="rId9" xr:uid="{79FD81E2-97EC-4684-88A0-EF6AAF32D284}"/>
-    <hyperlink ref="E24" r:id="rId10" xr:uid="{2241FBF8-050A-4F48-9C3A-490B16BED9AE}"/>
-    <hyperlink ref="E27" r:id="rId11" xr:uid="{E100ED19-A0C0-47BF-81B0-BF7A691C6E96}"/>
-    <hyperlink ref="E28" r:id="rId12" xr:uid="{09BB1505-958E-4E10-B12B-A8816FEA4E48}"/>
-    <hyperlink ref="E29" r:id="rId13" xr:uid="{BEDB1E05-168C-4E39-AE9B-3D546DC20298}"/>
-    <hyperlink ref="E30" r:id="rId14" xr:uid="{1C28DA7F-05B2-4158-8754-855124922569}"/>
-    <hyperlink ref="E14" r:id="rId15" xr:uid="{307AC36A-CB4F-4C22-A7BE-710EAFA5D473}"/>
-    <hyperlink ref="E7" r:id="rId16" xr:uid="{17A39F74-4FBC-4125-BEC9-4443E4E0CA1E}"/>
-    <hyperlink ref="E8" r:id="rId17" display="https://www.amazon.com/Creality-Filament-Printing-No-Tangling-Performance/dp/B0C6T3Y6SW/ref=sxin_16_pa_sp_search_thematic_sspa?content-id=amzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%3Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f&amp;cv_ct_cx=filament%2B3d%2Bprinting&amp;dib=eyJ2IjoiMSJ9.alyLMPbEnjPuo92a_LK93_jZ-GrR8invtSb7r3G1IWLlc-ip-tKUO_4uWDsxi5LNDZRh74Lt_FMRneqeD0My_w.fA5BQNJWm4ZdOPTeekItmjaooysuJCZP8KZRmhy0bFI&amp;dib_tag=se&amp;keywords=filament%2B3d%2Bprinting&amp;pd_rd_i=B0C4TNQZYY&amp;pd_rd_r=52d51348-04a5-41d5-b1ab-ee6ec080af13&amp;pd_rd_w=O4yN3&amp;pd_rd_wg=ZSQdf&amp;pf_rd_p=d4fdc453-1595-4f7b-ba6a-eb2ac554591f&amp;pf_rd_r=EBSTM6CYBWBGEAG9T600&amp;qid=1711740218&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sr=1-1-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM&amp;th=1" xr:uid="{CA49D3A1-65B3-4E57-8B92-37B02E722D31}"/>
-    <hyperlink ref="E12" r:id="rId18" display="https://www.amazon.com/TICONN-Clear-Safety-Glasses-Pack/dp/B0BGSFQJF6/ref=sr_1_2_sspa?crid=39460A9ZCG7Q0&amp;dib=eyJ2IjoiMSJ9.HBtZVdWaTQY4Lba_H8FXVSoRelAVSZSv5GgiYs-_uKK5YkeUUA13z4LVFxX5INVAI4EiBdEuPSvvWFXlhN3ghsfYNKPeLI5Z5PHnkkz5IT_4PZUOsjRPhWBwjs0sjjg2PicUS-bQrX_e8Y3EvnXuVuGAIArLKqcKPGdJLdIHE9-l3p69QpSOKeAtiitW-8w3CTOxTx_PcVGu6twA6qKrpcLcxw4f4i95lOmp-5AoDAlaClNkBjh6IBHVQgyohspE_DYw9BLm5xUWl9QW9ffKWFnE_PZY5tOg_GRHjnrQH8E.Pm0xFPQFbHQK9vUSzqvZZoxZ5QK9Rz7iXsUE_lcCKDU&amp;dib_tag=se&amp;keywords=safety+glasses&amp;qid=1711742295&amp;sprefix=safety+glasses%2Caps%2C182&amp;sr=8-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1" xr:uid="{D0641B11-3B03-486A-B8B9-8C7772931216}"/>
-    <hyperlink ref="E13" r:id="rId19" display="https://www.amazon.com/dp/B07Q2B4ZY9/ref=sspa_dk_detail_3?pf_rd_p=a53ea610-e450-44d1-897e-68c0c718bf50&amp;pf_rd_r=V7GFYD4F0J5FTDR0P5M1&amp;pd_rd_wg=8Thcb&amp;pd_rd_w=TXcNm&amp;content-id=amzn1.sym.a53ea610-e450-44d1-897e-68c0c718bf50&amp;pd_rd_r=21cb7e77-b095-4170-b779-0be4a698af56&amp;s=hi&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1" xr:uid="{F985562B-AFE6-40E8-9E63-043928BFED57}"/>
-    <hyperlink ref="E26" r:id="rId20" display="https://www.amazon.com/dp/B07Q2B4ZY9/ref=sspa_dk_detail_3?pf_rd_p=a53ea610-e450-44d1-897e-68c0c718bf50&amp;pf_rd_r=V7GFYD4F0J5FTDR0P5M1&amp;pd_rd_wg=8Thcb&amp;pd_rd_w=TXcNm&amp;content-id=amzn1.sym.a53ea610-e450-44d1-897e-68c0c718bf50&amp;pd_rd_r=21cb7e77-b095-4170-b779-0be4a698af56&amp;s=hi&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1" xr:uid="{1302B28C-6094-49D3-831F-3877547189F3}"/>
-    <hyperlink ref="E15" r:id="rId21" display="https://www.amazon.com/VELCRO-Brand-Mounting-Adhesive-Organization/dp/B099S34SVW/ref=sr_1_6?crid=3BA158YLBE8VK&amp;dib=eyJ2IjoiMSJ9.P9sHc2KKDrC-opAs_w3Pf4Ov0PupsO9oyxKPGRmHWCC4jBv6iAPR6Q4xqinlEkdYkyvYVsmJ15jwsYLu13GCqpm9BvpooCS8FXg-7ygtCrosVTp0feMW8kHzyomKa0hwdp0aN1Vc8NekLAt-7jV6YYkTj1ViVMbGkKaDatB--P1DECPyLpBODNX-Ih_QenaUQsHZ-7Ti0m2FT1msgEl48kAXSqyFKThv1CVCqOf2Fdp3fhJLdaYKMc8WMP2vM0StC9u3GGqgu-a1ktsepm-gakmZLNQJOVV12zTnJRHnuJw.0bLpGJQ9myRHIi8MOttStDYQ_bAf_DXU1N_VGFp6--s&amp;dib_tag=se&amp;keywords=velcro%2Bsquares%2Bwith%2Badhesive%2B1%2Binch&amp;qid=1711819467&amp;sprefix=velcro%2Bsquares%2Caps%2C147&amp;sr=8-6&amp;th=1" xr:uid="{FA2F3D62-CA42-4878-9560-692E6DE66E9A}"/>
-    <hyperlink ref="E17" r:id="rId22" display="https://www.amazon.com/Hillman-Group-59465-Machine-60-Pack/dp/B00NQQZSKW/ref=sr_1_3?crid=2HRNUBTOOJVQ8&amp;dib=eyJ2IjoiMSJ9.1vkNPU2FPrxW9nQjsWA0GIEM1WqYLllzRUv2SguZb535yiWfzbeh2ygAujyd3-PC4y7fjodf4U4nH0hqJ1ZXS-tu-tVX3wPyK02hsuawReAF1O8R6NkSwjMZb9mR-E5VuN8wqC1W7oHTMfXF2O30CJXKZeFwJw-544_vDHCypOadZxZWIG5d6mJorfdOFpFIzLx3y9scjGMUAAoUGMizN-amj502dAA17TfpfzzLllI.1J7Au9TBAztC4mU4NO2jxj1JQjZVRV4xTDsamQxQkTQ&amp;dib_tag=se&amp;keywords=4-40+nylon+screws+3%2F8&amp;qid=1711820811&amp;sprefix=4-40+nylon+screws+3%2F8%2Caps%2C126&amp;sr=8-3" xr:uid="{52E528F5-0EE9-4DED-BA40-E37C6FCCAD33}"/>
-    <hyperlink ref="E23" r:id="rId23" display="https://www.amazon.com/TICONN-Clear-Safety-Glasses-Pack/dp/B0BGSFQJF6/ref=sr_1_2_sspa?crid=39460A9ZCG7Q0&amp;dib=eyJ2IjoiMSJ9.HBtZVdWaTQY4Lba_H8FXVSoRelAVSZSv5GgiYs-_uKK5YkeUUA13z4LVFxX5INVAI4EiBdEuPSvvWFXlhN3ghsfYNKPeLI5Z5PHnkkz5IT_4PZUOsjRPhWBwjs0sjjg2PicUS-bQrX_e8Y3EvnXuVuGAIArLKqcKPGdJLdIHE9-l3p69QpSOKeAtiitW-8w3CTOxTx_PcVGu6twA6qKrpcLcxw4f4i95lOmp-5AoDAlaClNkBjh6IBHVQgyohspE_DYw9BLm5xUWl9QW9ffKWFnE_PZY5tOg_GRHjnrQH8E.Pm0xFPQFbHQK9vUSzqvZZoxZ5QK9Rz7iXsUE_lcCKDU&amp;dib_tag=se&amp;keywords=safety+glasses&amp;qid=1711742295&amp;sprefix=safety+glasses%2Caps%2C182&amp;sr=8-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1" xr:uid="{BF5DE3B8-9525-46C9-B617-FFCC45E39E3D}"/>
-    <hyperlink ref="E31" r:id="rId24" display="https://www.amazon.com/Pioneer-TS-F1634R-200W-2-Way-Speakers/dp/B0081SRIFS/ref=sr_1_3?crid=27GSO45Y8L89Y&amp;dib=eyJ2IjoiMSJ9.Qs7D6xm7evahvMLBO5d9b2C5TGd-VV9LfYSZ7XtH3jCkAXYGxT_DP9EoL-eSD14yN7RD6NHoPn3fESkoUw--aw7b0l9hanJwDuUgGsz2Cz7j_mthvFakvJqzMqmt397TIvwiM2dJyuKHG8igIKMKjqv162VxYVN-9ZC82i0qwd_5WNO0AyrRWZN0m2_k6VhXa1ISRHzuzh-wi6U9175ESpiyslqnQwq5TCV9HB8n-Iw.uhDUqm_1-84X0k2biGy6nL93Pdy4JuJWXsDHodJrUZk&amp;dib_tag=se&amp;keywords=car%2Bspeaker%2Bfull%2Brange&amp;qid=1711747374&amp;sprefix=car%2Bspeaker%2Bfull%2Brange%2Caps%2C155&amp;sr=8-3&amp;th=1" xr:uid="{22E4E957-51E7-4E53-8F13-DA6368AA17EB}"/>
-    <hyperlink ref="E35" r:id="rId25" display="https://www.amazon.com/Weller-SnPb-T0051403199-Lead-Solder/dp/B09LDG7J4L?pd_rd_w=YaLaq&amp;content-id=amzn1.sym.3c1bdb31-a20d-42d0-a8cf-ddadf63cd1a8&amp;pf_rd_p=3c1bdb31-a20d-42d0-a8cf-ddadf63cd1a8&amp;pf_rd_r=S8NBBKPB3CKZEN8EQSRS&amp;pd_rd_wg=BA5cI&amp;pd_rd_r=9183bcda-b054-4b06-9c62-1bea3eb2a208&amp;ref_=sspa_dk_detail_1&amp;th=1" xr:uid="{011E94FB-97C3-4F63-AE9B-40A7E84DF181}"/>
-    <hyperlink ref="E32" r:id="rId26" display="https://www.amazon.com/dp/B0BXT71WJK/?coliid=IEEB50BNR3XAR&amp;colid=29JXPO3FBZQZE&amp;ref_=list_c_wl_lv_ov_lig_dp_it&amp;th=1" xr:uid="{2A5FAADB-0752-485A-9AD3-4CC97E1BD712}"/>
-    <hyperlink ref="E34" r:id="rId27" display="https://www.amazon.com/Speaker-Stereo-Theater-Install-Link/dp/B0CLQV4BSH/ref=sr_1_3?crid=1RNCKDNFX958Y&amp;dib=eyJ2IjoiMSJ9.L_cSiPIT8KxNPj7xaUilvRMi89HtABjXwN40wBbWsYQqrkAmDhJNt2cJtaNSNVo3jqOTWesqXmy7oXmn64STMiNC9NAozH7LAT3UyrS1S5-qV9nDLQv2VydzJWRTqy6VhLFSysRgNx4uJ6F_j8AbGNncFabrsC4XrvxSBq-NbfWDRENp2fRMYq66HREHVZp6CQlLDIk2VaLXHm8aLOFZz-H3hhJDKrFIQAbn_wSwzvA.9xe9hd6t3fZHC_u9mcaGpfU5JtWjUVJDsnbp1NbHQqU&amp;dib_tag=se&amp;keywords=speaker%2Bwire&amp;qid=1712676542&amp;sprefix=speaker%2Bwire%2Caps%2C168&amp;sr=8-3&amp;th=1" xr:uid="{B7E52102-DB9E-48F4-9E08-D76DBA1EF9B7}"/>
-    <hyperlink ref="E33" r:id="rId28" display="https://www.amazon.com/Qibaok-Ratcheting-0-5-1-5mm%C2%B2-Connectors-Terminals/dp/B07RZSSTSJ/ref=sr_1_7_sspa?crid=1VPBVJKCTCX5V&amp;dib=eyJ2IjoiMSJ9.4apdw72O9qOi4VZRfFj7UilcADaLN50tuhFOrtrSXOHaaz2NmVWbDg_ZA17L-1wMItzTH8z6OQeF8YZBVTHZ172tmaMr_6lnypYgioksyD-Lo-6-4PHUf_1q20fD1eZZv0UWRHsHqzDnYZVZYzmTWnIJ1aLRAdZwH9vxRBlZ9RxENJiyKOb1-ahFcMRZoy-pGRewGtAc8grDq__o0Gfl3imnNPseqR3TEZYpX2NVwg8.OR7aXmWWUHMe6vaco7zOVKjBxUQGmqYE3p6XAxkSwgg&amp;dib_tag=se&amp;keywords=speaker+connector+kits&amp;qid=1712678957&amp;sprefix=speaker+connector+kits%2Caps%2C170&amp;sr=8-7-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9tdGY&amp;psc=1" xr:uid="{4CFE6712-C3C5-455F-963C-51F9EE4AECA9}"/>
-    <hyperlink ref="E21" r:id="rId29" xr:uid="{455F2275-D34C-46CA-B64D-6339CEB9BADF}"/>
-    <hyperlink ref="E2" r:id="rId30" xr:uid="{7C9C7DD4-1825-481D-AB53-D17266568F30}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{7BAAD23B-7678-4EBB-9B5A-661293E0F674}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{551F451C-DD03-4493-8EA8-59540528086E}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{25E4BF5A-A49F-480D-8849-CB7A7B9B79BE}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{A173BFB9-ABA9-4930-A528-581312F64ED0}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{1E8A2B7D-CC91-4B8A-8EA3-862EA551A3C4}"/>
+    <hyperlink ref="E11" r:id="rId6" display="https://www.amazon.com/Charger-Cabepow-Adapter-Replacement-Certified/dp/B09MRGLZ3W/ref=asc_df_B09MRGLZ3W/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=647232162671&amp;hvpos=&amp;hvnetw=g&amp;hvrand=8620124500595074403&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1016216&amp;hvtargid=pla-1950936299265&amp;mcid=efa7bf99c3543b43b3072f505e67ee13&amp;th=1" xr:uid="{F23F5859-01CD-4F5B-BC9E-C1111199B558}"/>
+    <hyperlink ref="E12" r:id="rId7" display="https://www.amazon.com/Charging-etguuds-Charger-Compatible-Samsung/dp/B089DM4KDW/ref=sr_1_3?crid=PM2LYP9121C&amp;dib=eyJ2IjoiMSJ9.XnJmpogYmdIy1CTZnxjk3yMJVv7eMnOaBQg168qPbg6U5oBzVS_uVzqHed3j6VZUslJKS891U51XQG6IZpFtGbDnRjf5leMIE9xP_5N2HFzCodmkJezSDly3v388XzfURpFN0ydF60pmJ1lZ-zB8nmVreFKbbjYd7UAbfLXusirgoToJLIWO26UszfL60F7HBmmGClCM5uaaSW1PcT_HPap0fMdBMz-B0UsPJVyDNOk.tPHZhfxNUqnfvIHsdn1pVZLA4syls-WTsZfRm-fcHQ8&amp;dib_tag=se&amp;keywords=usb%2Bc%2Bcable&amp;qid=1711749477&amp;sprefix=usb%2Bc%2Bcable%2Caps%2C146&amp;sr=8-3&amp;th=1" xr:uid="{85953D17-CC4C-4B91-8797-ED80017688ED}"/>
+    <hyperlink ref="E17" r:id="rId8" display="https://www.amazon.com/Stainless-Lengths-Available-Machine-Phillips/dp/B0793D86TB/ref=sr_1_21?crid=WBXT9P6GKIPF&amp;dib=eyJ2IjoiMSJ9.L6mfIE51zTPaywqeH0ar3jIX6WQ-gjM-wgJaUqgZeYVm5ChcscbE_zvlzc-lXdKwxf9_HO6jvI_KGoF38sNgFPWOSFrd3uGKhCrvjnYSEAaH61OiLBITDRwChiGXJiekfmtCUjgUL49s0s2umc79HVGfd0oocHT_SdOYOS862KFDrny6U2l-nYdirsQx8XNAaPfJXyXHHC71KG3dNjIx92lPwWic_wvQ3snGnakzY84.B7kH8YazXzMOwjwJAOCM1rgNsxzpzEb8TZWCjs78Xzc&amp;dib_tag=se&amp;keywords=6%2B32%2Bscrews&amp;qid=1711819989&amp;sprefix=6%2B32%2Bscrews%2Caps%2C132&amp;sr=8-21&amp;th=1" xr:uid="{E382410B-BB8A-4CFF-8C9E-BDC4985067E7}"/>
+    <hyperlink ref="E23" r:id="rId9" xr:uid="{79FD81E2-97EC-4684-88A0-EF6AAF32D284}"/>
+    <hyperlink ref="E25" r:id="rId10" xr:uid="{2241FBF8-050A-4F48-9C3A-490B16BED9AE}"/>
+    <hyperlink ref="E28" r:id="rId11" xr:uid="{E100ED19-A0C0-47BF-81B0-BF7A691C6E96}"/>
+    <hyperlink ref="E29" r:id="rId12" xr:uid="{09BB1505-958E-4E10-B12B-A8816FEA4E48}"/>
+    <hyperlink ref="E30" r:id="rId13" xr:uid="{BEDB1E05-168C-4E39-AE9B-3D546DC20298}"/>
+    <hyperlink ref="E31" r:id="rId14" xr:uid="{1C28DA7F-05B2-4158-8754-855124922569}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{307AC36A-CB4F-4C22-A7BE-710EAFA5D473}"/>
+    <hyperlink ref="E8" r:id="rId16" xr:uid="{17A39F74-4FBC-4125-BEC9-4443E4E0CA1E}"/>
+    <hyperlink ref="E9" r:id="rId17" display="https://www.amazon.com/Creality-Filament-Printing-No-Tangling-Performance/dp/B0C6T3Y6SW/ref=sxin_16_pa_sp_search_thematic_sspa?content-id=amzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%3Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f&amp;cv_ct_cx=filament%2B3d%2Bprinting&amp;dib=eyJ2IjoiMSJ9.alyLMPbEnjPuo92a_LK93_jZ-GrR8invtSb7r3G1IWLlc-ip-tKUO_4uWDsxi5LNDZRh74Lt_FMRneqeD0My_w.fA5BQNJWm4ZdOPTeekItmjaooysuJCZP8KZRmhy0bFI&amp;dib_tag=se&amp;keywords=filament%2B3d%2Bprinting&amp;pd_rd_i=B0C4TNQZYY&amp;pd_rd_r=52d51348-04a5-41d5-b1ab-ee6ec080af13&amp;pd_rd_w=O4yN3&amp;pd_rd_wg=ZSQdf&amp;pf_rd_p=d4fdc453-1595-4f7b-ba6a-eb2ac554591f&amp;pf_rd_r=EBSTM6CYBWBGEAG9T600&amp;qid=1711740218&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sr=1-1-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM&amp;th=1" xr:uid="{CA49D3A1-65B3-4E57-8B92-37B02E722D31}"/>
+    <hyperlink ref="E13" r:id="rId18" display="https://www.amazon.com/TICONN-Clear-Safety-Glasses-Pack/dp/B0BGSFQJF6/ref=sr_1_2_sspa?crid=39460A9ZCG7Q0&amp;dib=eyJ2IjoiMSJ9.HBtZVdWaTQY4Lba_H8FXVSoRelAVSZSv5GgiYs-_uKK5YkeUUA13z4LVFxX5INVAI4EiBdEuPSvvWFXlhN3ghsfYNKPeLI5Z5PHnkkz5IT_4PZUOsjRPhWBwjs0sjjg2PicUS-bQrX_e8Y3EvnXuVuGAIArLKqcKPGdJLdIHE9-l3p69QpSOKeAtiitW-8w3CTOxTx_PcVGu6twA6qKrpcLcxw4f4i95lOmp-5AoDAlaClNkBjh6IBHVQgyohspE_DYw9BLm5xUWl9QW9ffKWFnE_PZY5tOg_GRHjnrQH8E.Pm0xFPQFbHQK9vUSzqvZZoxZ5QK9Rz7iXsUE_lcCKDU&amp;dib_tag=se&amp;keywords=safety+glasses&amp;qid=1711742295&amp;sprefix=safety+glasses%2Caps%2C182&amp;sr=8-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1" xr:uid="{D0641B11-3B03-486A-B8B9-8C7772931216}"/>
+    <hyperlink ref="E14" r:id="rId19" display="https://www.amazon.com/dp/B07Q2B4ZY9/ref=sspa_dk_detail_3?pf_rd_p=a53ea610-e450-44d1-897e-68c0c718bf50&amp;pf_rd_r=V7GFYD4F0J5FTDR0P5M1&amp;pd_rd_wg=8Thcb&amp;pd_rd_w=TXcNm&amp;content-id=amzn1.sym.a53ea610-e450-44d1-897e-68c0c718bf50&amp;pd_rd_r=21cb7e77-b095-4170-b779-0be4a698af56&amp;s=hi&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1" xr:uid="{F985562B-AFE6-40E8-9E63-043928BFED57}"/>
+    <hyperlink ref="E27" r:id="rId20" display="https://www.amazon.com/dp/B07Q2B4ZY9/ref=sspa_dk_detail_3?pf_rd_p=a53ea610-e450-44d1-897e-68c0c718bf50&amp;pf_rd_r=V7GFYD4F0J5FTDR0P5M1&amp;pd_rd_wg=8Thcb&amp;pd_rd_w=TXcNm&amp;content-id=amzn1.sym.a53ea610-e450-44d1-897e-68c0c718bf50&amp;pd_rd_r=21cb7e77-b095-4170-b779-0be4a698af56&amp;s=hi&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1" xr:uid="{1302B28C-6094-49D3-831F-3877547189F3}"/>
+    <hyperlink ref="E16" r:id="rId21" display="https://www.amazon.com/VELCRO-Brand-Mounting-Adhesive-Organization/dp/B099S34SVW/ref=sr_1_6?crid=3BA158YLBE8VK&amp;dib=eyJ2IjoiMSJ9.P9sHc2KKDrC-opAs_w3Pf4Ov0PupsO9oyxKPGRmHWCC4jBv6iAPR6Q4xqinlEkdYkyvYVsmJ15jwsYLu13GCqpm9BvpooCS8FXg-7ygtCrosVTp0feMW8kHzyomKa0hwdp0aN1Vc8NekLAt-7jV6YYkTj1ViVMbGkKaDatB--P1DECPyLpBODNX-Ih_QenaUQsHZ-7Ti0m2FT1msgEl48kAXSqyFKThv1CVCqOf2Fdp3fhJLdaYKMc8WMP2vM0StC9u3GGqgu-a1ktsepm-gakmZLNQJOVV12zTnJRHnuJw.0bLpGJQ9myRHIi8MOttStDYQ_bAf_DXU1N_VGFp6--s&amp;dib_tag=se&amp;keywords=velcro%2Bsquares%2Bwith%2Badhesive%2B1%2Binch&amp;qid=1711819467&amp;sprefix=velcro%2Bsquares%2Caps%2C147&amp;sr=8-6&amp;th=1" xr:uid="{FA2F3D62-CA42-4878-9560-692E6DE66E9A}"/>
+    <hyperlink ref="E18" r:id="rId22" display="https://www.amazon.com/Hillman-Group-59465-Machine-60-Pack/dp/B00NQQZSKW/ref=sr_1_3?crid=2HRNUBTOOJVQ8&amp;dib=eyJ2IjoiMSJ9.1vkNPU2FPrxW9nQjsWA0GIEM1WqYLllzRUv2SguZb535yiWfzbeh2ygAujyd3-PC4y7fjodf4U4nH0hqJ1ZXS-tu-tVX3wPyK02hsuawReAF1O8R6NkSwjMZb9mR-E5VuN8wqC1W7oHTMfXF2O30CJXKZeFwJw-544_vDHCypOadZxZWIG5d6mJorfdOFpFIzLx3y9scjGMUAAoUGMizN-amj502dAA17TfpfzzLllI.1J7Au9TBAztC4mU4NO2jxj1JQjZVRV4xTDsamQxQkTQ&amp;dib_tag=se&amp;keywords=4-40+nylon+screws+3%2F8&amp;qid=1711820811&amp;sprefix=4-40+nylon+screws+3%2F8%2Caps%2C126&amp;sr=8-3" xr:uid="{52E528F5-0EE9-4DED-BA40-E37C6FCCAD33}"/>
+    <hyperlink ref="E24" r:id="rId23" display="https://www.amazon.com/TICONN-Clear-Safety-Glasses-Pack/dp/B0BGSFQJF6/ref=sr_1_2_sspa?crid=39460A9ZCG7Q0&amp;dib=eyJ2IjoiMSJ9.HBtZVdWaTQY4Lba_H8FXVSoRelAVSZSv5GgiYs-_uKK5YkeUUA13z4LVFxX5INVAI4EiBdEuPSvvWFXlhN3ghsfYNKPeLI5Z5PHnkkz5IT_4PZUOsjRPhWBwjs0sjjg2PicUS-bQrX_e8Y3EvnXuVuGAIArLKqcKPGdJLdIHE9-l3p69QpSOKeAtiitW-8w3CTOxTx_PcVGu6twA6qKrpcLcxw4f4i95lOmp-5AoDAlaClNkBjh6IBHVQgyohspE_DYw9BLm5xUWl9QW9ffKWFnE_PZY5tOg_GRHjnrQH8E.Pm0xFPQFbHQK9vUSzqvZZoxZ5QK9Rz7iXsUE_lcCKDU&amp;dib_tag=se&amp;keywords=safety+glasses&amp;qid=1711742295&amp;sprefix=safety+glasses%2Caps%2C182&amp;sr=8-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1" xr:uid="{BF5DE3B8-9525-46C9-B617-FFCC45E39E3D}"/>
+    <hyperlink ref="E32" r:id="rId24" display="https://www.amazon.com/Pioneer-TS-F1634R-200W-2-Way-Speakers/dp/B0081SRIFS/ref=sr_1_3?crid=27GSO45Y8L89Y&amp;dib=eyJ2IjoiMSJ9.Qs7D6xm7evahvMLBO5d9b2C5TGd-VV9LfYSZ7XtH3jCkAXYGxT_DP9EoL-eSD14yN7RD6NHoPn3fESkoUw--aw7b0l9hanJwDuUgGsz2Cz7j_mthvFakvJqzMqmt397TIvwiM2dJyuKHG8igIKMKjqv162VxYVN-9ZC82i0qwd_5WNO0AyrRWZN0m2_k6VhXa1ISRHzuzh-wi6U9175ESpiyslqnQwq5TCV9HB8n-Iw.uhDUqm_1-84X0k2biGy6nL93Pdy4JuJWXsDHodJrUZk&amp;dib_tag=se&amp;keywords=car%2Bspeaker%2Bfull%2Brange&amp;qid=1711747374&amp;sprefix=car%2Bspeaker%2Bfull%2Brange%2Caps%2C155&amp;sr=8-3&amp;th=1" xr:uid="{22E4E957-51E7-4E53-8F13-DA6368AA17EB}"/>
+    <hyperlink ref="E36" r:id="rId25" display="https://www.amazon.com/Weller-SnPb-T0051403199-Lead-Solder/dp/B09LDG7J4L?pd_rd_w=YaLaq&amp;content-id=amzn1.sym.3c1bdb31-a20d-42d0-a8cf-ddadf63cd1a8&amp;pf_rd_p=3c1bdb31-a20d-42d0-a8cf-ddadf63cd1a8&amp;pf_rd_r=S8NBBKPB3CKZEN8EQSRS&amp;pd_rd_wg=BA5cI&amp;pd_rd_r=9183bcda-b054-4b06-9c62-1bea3eb2a208&amp;ref_=sspa_dk_detail_1&amp;th=1" xr:uid="{011E94FB-97C3-4F63-AE9B-40A7E84DF181}"/>
+    <hyperlink ref="E33" r:id="rId26" display="https://www.amazon.com/dp/B0BXT71WJK/?coliid=IEEB50BNR3XAR&amp;colid=29JXPO3FBZQZE&amp;ref_=list_c_wl_lv_ov_lig_dp_it&amp;th=1" xr:uid="{2A5FAADB-0752-485A-9AD3-4CC97E1BD712}"/>
+    <hyperlink ref="E35" r:id="rId27" display="https://www.amazon.com/Speaker-Stereo-Theater-Install-Link/dp/B0CLQV4BSH/ref=sr_1_3?crid=1RNCKDNFX958Y&amp;dib=eyJ2IjoiMSJ9.L_cSiPIT8KxNPj7xaUilvRMi89HtABjXwN40wBbWsYQqrkAmDhJNt2cJtaNSNVo3jqOTWesqXmy7oXmn64STMiNC9NAozH7LAT3UyrS1S5-qV9nDLQv2VydzJWRTqy6VhLFSysRgNx4uJ6F_j8AbGNncFabrsC4XrvxSBq-NbfWDRENp2fRMYq66HREHVZp6CQlLDIk2VaLXHm8aLOFZz-H3hhJDKrFIQAbn_wSwzvA.9xe9hd6t3fZHC_u9mcaGpfU5JtWjUVJDsnbp1NbHQqU&amp;dib_tag=se&amp;keywords=speaker%2Bwire&amp;qid=1712676542&amp;sprefix=speaker%2Bwire%2Caps%2C168&amp;sr=8-3&amp;th=1" xr:uid="{B7E52102-DB9E-48F4-9E08-D76DBA1EF9B7}"/>
+    <hyperlink ref="E34" r:id="rId28" display="https://www.amazon.com/Qibaok-Ratcheting-0-5-1-5mm%C2%B2-Connectors-Terminals/dp/B07RZSSTSJ/ref=sr_1_7_sspa?crid=1VPBVJKCTCX5V&amp;dib=eyJ2IjoiMSJ9.4apdw72O9qOi4VZRfFj7UilcADaLN50tuhFOrtrSXOHaaz2NmVWbDg_ZA17L-1wMItzTH8z6OQeF8YZBVTHZ172tmaMr_6lnypYgioksyD-Lo-6-4PHUf_1q20fD1eZZv0UWRHsHqzDnYZVZYzmTWnIJ1aLRAdZwH9vxRBlZ9RxENJiyKOb1-ahFcMRZoy-pGRewGtAc8grDq__o0Gfl3imnNPseqR3TEZYpX2NVwg8.OR7aXmWWUHMe6vaco7zOVKjBxUQGmqYE3p6XAxkSwgg&amp;dib_tag=se&amp;keywords=speaker+connector+kits&amp;qid=1712678957&amp;sprefix=speaker+connector+kits%2Caps%2C170&amp;sr=8-7-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9tdGY&amp;psc=1" xr:uid="{4CFE6712-C3C5-455F-963C-51F9EE4AECA9}"/>
+    <hyperlink ref="E22" r:id="rId29" xr:uid="{455F2275-D34C-46CA-B64D-6339CEB9BADF}"/>
+    <hyperlink ref="E3" r:id="rId30" xr:uid="{7C9C7DD4-1825-481D-AB53-D17266568F30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>